<commit_message>
Landkreise überarbeitet als file + md, updates in Schema-Doku
</commit_message>
<xml_diff>
--- a/oBDS_v3.0.0.8a_RKI_Schema.xlsx
+++ b/oBDS_v3.0.0.8a_RKI_Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\4_Daten\Onkodaten\Klassifikationen Datensatz 2023\__Arbeitsdokumente ZfKD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF868B7-7102-483A-8456-E53DC8D52F92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A7A9EF-5881-4B6C-AB39-B050FFF1F529}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="6990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="886">
   <si>
     <t>Variablen-Nr</t>
   </si>
@@ -1015,15 +1015,9 @@
     <t>DCN</t>
   </si>
   <si>
-    <t>Gibt an, ob die Todesbescheinigung die erste Informationsquelle zu einem Erkrankungsfall war. Handelt es sich um einen DCO-Fall, ist DCN = Ja unplausibel.</t>
-  </si>
-  <si>
     <t>Death certificate notified (DCN)</t>
   </si>
   <si>
-    <t>Indicates whether or not the case was first notified by a death certificate. For DCO cases, DCN = Yes is not plausible.</t>
-  </si>
-  <si>
     <t>Anzahl_Tage_Diagnose_Tod</t>
   </si>
   <si>
@@ -1216,9 +1210,6 @@
     <t>2, 3, 4, 5, 6, 7, 7a, 7b, 8, 9 oder 10</t>
   </si>
   <si>
-    <t>Gleason: score</t>
-  </si>
-  <si>
     <t>Gleason score</t>
   </si>
   <si>
@@ -1229,12 +1220,6 @@
   </si>
   <si>
     <t>Gleason-Score Anlass</t>
-  </si>
-  <si>
-    <t>Gleason: sampling method</t>
-  </si>
-  <si>
-    <t>Sampling method</t>
   </si>
   <si>
     <t>Primärdiagnose: Modul Melanom</t>
@@ -1544,9 +1529,6 @@
     <t>Describes percutaneous radiotherapy (external beam radiotherapy) target site according to oBDS v2014.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>CodeVersion2021</t>
   </si>
   <si>
@@ -1571,26 +1553,10 @@
     <t>Bezeichnet die Körperseite der behandelten anatomischen Region.</t>
   </si>
   <si>
-    <t>L = links
-R = rechts
-B = beidseits
-M = mittig
-U = unbekannt
-T = trifft nicht zu</t>
-  </si>
-  <si>
     <t>Percutaneous radiotherapy - laterality</t>
   </si>
   <si>
     <t>Describes laterality of percutaneous radiotherapy (external beam radiotherapy) target site.</t>
-  </si>
-  <si>
-    <t>L = left
-R = right
-B = bilateral
-M = center
-U = unknown
-T = not applicable</t>
   </si>
   <si>
     <t>Interstitiell_endokavitaer</t>
@@ -2123,9 +2089,6 @@
   </si>
   <si>
     <t>Gesamtbeurteilung_Tumorstatus</t>
-  </si>
-  <si>
-    <t>Gesamtburteilung Tumorstatus</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamtbeurteilung der Erkrankung unter Berücksichtigung aller Manifestationen. </t>
@@ -3603,9 +3566,6 @@
     <t>Gleason-Score.</t>
   </si>
   <si>
-    <t>Methode der Probenahme.</t>
-  </si>
-  <si>
     <t>Tumordicke (in mm).</t>
   </si>
   <si>
@@ -3667,6 +3627,58 @@
   </si>
   <si>
     <t>Beurteilung der Situation im Bereich der Fernmetastasen. "R" beschreibt eine Situation, in der zuvor Metastasenfreiheit bestanden hat oder durch Therapie erreicht wurde. "P" beschreibt neu hinzukommende (zu bereits bestehenden) Fernmetastasen.</t>
+  </si>
+  <si>
+    <t>Gesamtbeurteilung Tumorstatus</t>
+  </si>
+  <si>
+    <t>Anlass der Bestimmung.</t>
+  </si>
+  <si>
+    <t>Gibt an, ob die Quelle der ersten Information über einen Erkrankungsfall im Register eine Todesbescheinigung bzw. eine amtlich übermittelte Todesursache war.</t>
+  </si>
+  <si>
+    <t>Indicates whether or not the case was first notified by death certificate (official cause of death).</t>
+  </si>
+  <si>
+    <t>Gleason score: sampling method</t>
+  </si>
+  <si>
+    <t>Describes tissue sampling method/origin of tissue sample used to determine Gleason score.</t>
+  </si>
+  <si>
+    <t>(name) = protocol name</t>
+  </si>
+  <si>
+    <t>(version) = protocol version</t>
+  </si>
+  <si>
+    <t>(Name, Typ) = Bezeichnung des Klassifikationssystems, z. B. Ann-Arbor-Klassifikation, WHO Classification of CNS Tumors, AJCC</t>
+  </si>
+  <si>
+    <t>(Stadium) = Stadium gemäß verwendetem Klassifikationssystem</t>
+  </si>
+  <si>
+    <t>L = links;
+R = rechts;
+B = beidseits;
+M = mittig;
+U = unbekannt;
+T = trifft nicht zu</t>
+  </si>
+  <si>
+    <t>L = left; 
+R = right;
+B = bilateral;
+M = center;
+U = unknown;
+T = not applicable</t>
+  </si>
+  <si>
+    <t>(Protokoll) = Bezeichnung des Therapieprotokolls</t>
+  </si>
+  <si>
+    <t>(Version) = Version des verwendeten Therapieprotokolls</t>
   </si>
 </sst>
 </file>
@@ -3730,24 +3742,6 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3837,6 +3831,24 @@
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3869,18 +3881,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="oBDS_v3_0_0_8a_RKI_Schema" displayName="oBDS_v3_0_0_8a_RKI_Schema" ref="A1:I156" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="oBDS_v3_0_0_8a_RKI_Schema" displayName="oBDS_v3_0_0_8a_RKI_Schema" ref="A1:I156" tableType="queryTable" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I156" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Variablen-Nr" queryTableFieldId="1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Gehört zu" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Variable (technische Bezeichnung)" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Variable" queryTableFieldId="4" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Beschreibung" queryTableFieldId="5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Ausprägungen" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Variable (English)" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Description" queryTableFieldId="8" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Value range" queryTableFieldId="9" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Variablen-Nr" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Gehört zu" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Variable (technische Bezeichnung)" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Variable" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Beschreibung" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Ausprägungen" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Variable (English)" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Description" queryTableFieldId="8" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Value range" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4185,8 +4197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4249,7 +4261,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -4258,7 +4270,7 @@
         <v>12</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4275,19 +4287,19 @@
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4336,7 +4348,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>25</v>
@@ -4345,7 +4357,7 @@
         <v>26</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4362,19 +4374,19 @@
         <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4420,19 +4432,19 @@
         <v>37</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4507,19 +4519,19 @@
         <v>55</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4597,7 +4609,7 @@
         <v>68</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>69</v>
@@ -4606,7 +4618,7 @@
         <v>70</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="270" x14ac:dyDescent="0.25">
@@ -4626,7 +4638,7 @@
         <v>73</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>74</v>
@@ -4635,7 +4647,7 @@
         <v>75</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4800,7 +4812,7 @@
         <v>111</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>112</v>
@@ -4809,7 +4821,7 @@
         <v>113</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4858,7 +4870,7 @@
         <v>123</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>124</v>
@@ -4867,7 +4879,7 @@
         <v>125</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -4887,7 +4899,7 @@
         <v>127</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>128</v>
@@ -4896,7 +4908,7 @@
         <v>129</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -4913,7 +4925,7 @@
         <v>131</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>132</v>
@@ -4942,7 +4954,7 @@
         <v>137</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>132</v>
@@ -4974,7 +4986,7 @@
         <v>142</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>143</v>
@@ -4983,7 +4995,7 @@
         <v>144</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5003,7 +5015,7 @@
         <v>147</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>148</v>
@@ -5148,7 +5160,7 @@
         <v>181</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>182</v>
@@ -5157,10 +5169,10 @@
         <v>183</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5177,7 +5189,7 @@
         <v>186</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>187</v>
@@ -5186,10 +5198,10 @@
         <v>188</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5206,7 +5218,7 @@
         <v>191</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>192</v>
@@ -5215,10 +5227,10 @@
         <v>193</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5235,7 +5247,7 @@
         <v>196</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>742</v>
+        <v>733</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>197</v>
@@ -5244,7 +5256,7 @@
         <v>198</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>741</v>
+        <v>732</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5264,7 +5276,7 @@
         <v>201</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>743</v>
+        <v>734</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>202</v>
@@ -5273,7 +5285,7 @@
         <v>203</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>744</v>
+        <v>735</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5293,7 +5305,7 @@
         <v>206</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>746</v>
+        <v>737</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>207</v>
@@ -5302,7 +5314,7 @@
         <v>208</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5322,7 +5334,7 @@
         <v>211</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>747</v>
+        <v>738</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>212</v>
@@ -5331,7 +5343,7 @@
         <v>213</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>748</v>
+        <v>739</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5351,7 +5363,7 @@
         <v>216</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>750</v>
+        <v>741</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>217</v>
@@ -5360,7 +5372,7 @@
         <v>218</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>749</v>
+        <v>740</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5380,7 +5392,7 @@
         <v>221</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>751</v>
+        <v>742</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>222</v>
@@ -5389,7 +5401,7 @@
         <v>223</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>752</v>
+        <v>743</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5438,7 +5450,7 @@
         <v>233</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>234</v>
@@ -5447,7 +5459,7 @@
         <v>235</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5496,7 +5508,7 @@
         <v>245</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>753</v>
+        <v>744</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>246</v>
@@ -5505,7 +5517,7 @@
         <v>247</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5525,7 +5537,7 @@
         <v>250</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>756</v>
+        <v>747</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>251</v>
@@ -5534,7 +5546,7 @@
         <v>252</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5612,7 +5624,7 @@
         <v>181</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>261</v>
@@ -5621,10 +5633,10 @@
         <v>262</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -5641,7 +5653,7 @@
         <v>186</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>759</v>
+        <v>750</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>265</v>
@@ -5650,7 +5662,7 @@
         <v>266</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5670,7 +5682,7 @@
         <v>191</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>269</v>
@@ -5679,7 +5691,7 @@
         <v>270</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>761</v>
+        <v>752</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5699,7 +5711,7 @@
         <v>196</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>763</v>
+        <v>754</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>273</v>
@@ -5708,7 +5720,7 @@
         <v>274</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5728,7 +5740,7 @@
         <v>201</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>764</v>
+        <v>755</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>277</v>
@@ -5737,7 +5749,7 @@
         <v>203</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5757,7 +5769,7 @@
         <v>280</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>767</v>
+        <v>758</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>281</v>
@@ -5766,7 +5778,7 @@
         <v>282</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>766</v>
+        <v>757</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5786,7 +5798,7 @@
         <v>285</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>768</v>
+        <v>759</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>286</v>
@@ -5795,7 +5807,7 @@
         <v>287</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5815,7 +5827,7 @@
         <v>290</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>291</v>
@@ -5824,7 +5836,7 @@
         <v>218</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5844,7 +5856,7 @@
         <v>221</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>294</v>
@@ -5853,7 +5865,7 @@
         <v>223</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>773</v>
+        <v>764</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5902,7 +5914,7 @@
         <v>300</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>774</v>
+        <v>765</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>301</v>
@@ -5911,7 +5923,7 @@
         <v>302</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>775</v>
+        <v>766</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -5928,10 +5940,10 @@
         <v>304</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>305</v>
+        <v>880</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>306</v>
@@ -5957,10 +5969,10 @@
         <v>310</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>309</v>
+        <v>881</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>311</v>
@@ -5986,10 +5998,10 @@
         <v>314</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>854</v>
+        <v>845</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>777</v>
+        <v>768</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>315</v>
@@ -5998,7 +6010,7 @@
         <v>316</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>776</v>
+        <v>767</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6018,7 +6030,7 @@
         <v>319</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>778</v>
+        <v>769</v>
       </c>
       <c r="G63" s="6" t="s">
         <v>320</v>
@@ -6027,7 +6039,7 @@
         <v>321</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>779</v>
+        <v>770</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6044,19 +6056,19 @@
         <v>322</v>
       </c>
       <c r="E64" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="G64" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="F64" s="7" t="s">
-        <v>713</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>324</v>
-      </c>
       <c r="H64" s="7" t="s">
-        <v>325</v>
+        <v>875</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -6067,25 +6079,25 @@
         <v>53</v>
       </c>
       <c r="C65" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E65" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="F65" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="G65" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="H65" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="I65" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -6093,28 +6105,28 @@
         <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="E66" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="F66" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="G66" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>781</v>
-      </c>
-      <c r="F66" s="6" t="s">
+      <c r="H66" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="G66" s="6" t="s">
+      <c r="I66" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="I66" s="6" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -6122,28 +6134,28 @@
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C67" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="F67" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="G67" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="E67" s="7" t="s">
-        <v>780</v>
-      </c>
-      <c r="F67" s="6" t="s">
+      <c r="H67" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="G67" s="6" t="s">
+      <c r="I67" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6151,28 +6163,28 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C68" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="F68" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="G68" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="E68" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>784</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>349</v>
-      </c>
       <c r="H68" s="7" t="s">
-        <v>783</v>
+        <v>774</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>782</v>
+        <v>773</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6180,28 +6192,28 @@
         <v>68</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C69" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="G69" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="H69" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="E69" s="7" t="s">
-        <v>786</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>785</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>353</v>
-      </c>
       <c r="I69" s="7" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6209,28 +6221,28 @@
         <v>69</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="G70" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="H70" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="E70" s="7" t="s">
-        <v>788</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>785</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="H70" s="7" t="s">
-        <v>357</v>
-      </c>
       <c r="I70" s="7" t="s">
-        <v>787</v>
+        <v>778</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6238,28 +6250,28 @@
         <v>70</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C71" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="E71" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="F71" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="F71" s="7" t="s">
-        <v>789</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>362</v>
-      </c>
       <c r="I71" s="7" t="s">
-        <v>790</v>
+        <v>781</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -6267,28 +6279,28 @@
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="E72" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="F72" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="G72" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="E72" s="7" t="s">
-        <v>855</v>
-      </c>
-      <c r="F72" s="6" t="s">
+      <c r="H72" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="G72" s="6" t="s">
+      <c r="I72" s="6" t="s">
         <v>367</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="I72" s="6" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -6296,28 +6308,28 @@
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C73" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="G73" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="D73" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>720</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>710</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>372</v>
-      </c>
       <c r="H73" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -6325,25 +6337,25 @@
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>21</v>
@@ -6354,28 +6366,28 @@
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C75" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="F75" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="G75" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="E75" s="7" t="s">
-        <v>857</v>
-      </c>
-      <c r="F75" s="6" t="s">
+      <c r="H75" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="G75" s="6" t="s">
+      <c r="I75" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="I75" s="6" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -6383,28 +6395,28 @@
         <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C76" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="G76" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="H76" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="E76" s="7" t="s">
-        <v>858</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>386</v>
-      </c>
       <c r="I76" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -6412,28 +6424,28 @@
         <v>76</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C77" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="F77" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="G77" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="E77" s="7" t="s">
-        <v>859</v>
-      </c>
-      <c r="F77" s="6" t="s">
+      <c r="H77" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="I77" s="6" t="s">
         <v>389</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6441,28 +6453,28 @@
         <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>860</v>
+        <v>873</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>395</v>
+        <v>876</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>396</v>
+        <v>877</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>791</v>
+        <v>782</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -6470,28 +6482,28 @@
         <v>78</v>
       </c>
       <c r="B79" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="H79" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="I79" s="6" t="s">
         <v>398</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>861</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="I79" s="6" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6499,28 +6511,28 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -6528,28 +6540,28 @@
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>862</v>
+        <v>852</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="I81" s="6" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6557,28 +6569,28 @@
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="H82" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="C82" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>794</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>418</v>
-      </c>
       <c r="I82" s="7" t="s">
-        <v>793</v>
+        <v>784</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6586,28 +6598,28 @@
         <v>82</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>796</v>
+        <v>787</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -6615,28 +6627,28 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6644,25 +6656,25 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="D85" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>429</v>
-      </c>
       <c r="E85" s="7" t="s">
-        <v>863</v>
+        <v>853</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="I85" s="6" t="s">
         <v>21</v>
@@ -6673,28 +6685,28 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>864</v>
+        <v>854</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -6702,28 +6714,28 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>865</v>
+        <v>855</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6731,28 +6743,28 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>798</v>
+        <v>789</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I88" s="7" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -6760,28 +6772,28 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="I89" s="7" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6789,28 +6801,28 @@
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>866</v>
+        <v>856</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -6818,28 +6830,28 @@
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I91" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -6847,25 +6859,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="C92" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>461</v>
-      </c>
       <c r="E92" s="7" t="s">
-        <v>867</v>
+        <v>857</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="I92" s="6" t="s">
         <v>21</v>
@@ -6876,28 +6888,28 @@
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6905,28 +6917,28 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -6934,28 +6946,28 @@
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="I95" s="7" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6963,28 +6975,28 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6992,28 +7004,28 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C97" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="H97" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="I97" s="6" t="s">
         <v>481</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="I97" s="6" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7021,28 +7033,28 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="H98" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="I98" s="6" t="s">
         <v>488</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="G98" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="H98" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="I98" s="6" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7050,28 +7062,28 @@
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="I99" s="7" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7079,28 +7091,28 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="I100" s="7" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7108,28 +7120,28 @@
         <v>100</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="I101" s="7" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7137,28 +7149,28 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>817</v>
+        <v>808</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -7166,28 +7178,28 @@
         <v>102</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>818</v>
+        <v>809</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7195,28 +7207,28 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7224,28 +7236,28 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="I105" s="7" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7253,28 +7265,28 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -7282,28 +7294,28 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>819</v>
+        <v>810</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7311,28 +7323,28 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="I108" s="7" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7340,57 +7352,57 @@
         <v>108</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="I109" s="7" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>508</v>
+        <v>501</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>882</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="I110" s="6" t="s">
-        <v>511</v>
+        <v>535</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7398,28 +7410,28 @@
         <v>110</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="I111" s="7" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7427,28 +7439,28 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="I112" s="7" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7456,28 +7468,28 @@
         <v>112</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7485,28 +7497,28 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -7514,28 +7526,28 @@
         <v>114</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7543,28 +7555,28 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="I116" s="7" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7572,28 +7584,28 @@
         <v>116</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -7601,28 +7613,28 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="I118" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -7630,28 +7642,28 @@
         <v>118</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>869</v>
+        <v>859</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="I119" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7659,28 +7671,28 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="I120" s="7" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -7688,28 +7700,28 @@
         <v>120</v>
       </c>
       <c r="B121" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="H121" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="C121" s="6" t="s">
-        <v>465</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="F121" s="7" t="s">
-        <v>848</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>576</v>
-      </c>
-      <c r="H121" s="7" t="s">
-        <v>577</v>
-      </c>
       <c r="I121" s="7" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -7717,28 +7729,28 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="I122" s="7" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7746,28 +7758,28 @@
         <v>122</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -7775,28 +7787,28 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="I124" s="6" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -7804,28 +7816,28 @@
         <v>124</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>871</v>
+        <v>861</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>834</v>
+        <v>825</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="I125" s="6" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -7833,82 +7845,86 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>870</v>
+        <v>860</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>499</v>
+        <v>884</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="I126" s="6"/>
+        <v>594</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>873</v>
+        <v>863</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>499</v>
+        <v>885</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H127" s="7" t="s">
-        <v>605</v>
-      </c>
-      <c r="I127" s="6"/>
+        <v>597</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="128" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F128" s="7" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I128" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -7916,25 +7932,25 @@
         <v>128</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>874</v>
+        <v>864</v>
       </c>
       <c r="F129" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="I129" s="6" t="s">
         <v>21</v>
@@ -7945,28 +7961,28 @@
         <v>129</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>875</v>
+        <v>865</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="I130" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7974,28 +7990,28 @@
         <v>130</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="I131" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -8003,28 +8019,28 @@
         <v>131</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="I132" s="7" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -8032,25 +8048,25 @@
         <v>132</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="F133" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="I133" s="6" t="s">
         <v>21</v>
@@ -8061,28 +8077,28 @@
         <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>846</v>
+        <v>837</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="I134" s="7" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -8090,28 +8106,28 @@
         <v>134</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>845</v>
+        <v>836</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="H135" s="7" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="I135" s="7" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8119,28 +8135,28 @@
         <v>135</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="F136" s="7" t="s">
-        <v>753</v>
+        <v>744</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="H136" s="7" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="I136" s="7" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8148,28 +8164,28 @@
         <v>136</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="F137" s="7" t="s">
-        <v>756</v>
+        <v>747</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="H137" s="7" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="I137" s="7" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8177,13 +8193,13 @@
         <v>137</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E138" s="7" t="s">
         <v>167</v>
@@ -8192,7 +8208,7 @@
         <v>168</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="H138" s="7" t="s">
         <v>170</v>
@@ -8206,13 +8222,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="E139" s="7" t="s">
         <v>174</v>
@@ -8221,7 +8237,7 @@
         <v>175</v>
       </c>
       <c r="G139" s="6" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="H139" s="7" t="s">
         <v>177</v>
@@ -8235,28 +8251,28 @@
         <v>139</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>181</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>844</v>
+        <v>835</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="H140" s="7" t="s">
         <v>262</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>757</v>
+        <v>748</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8264,28 +8280,28 @@
         <v>140</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="E141" s="7" t="s">
         <v>186</v>
       </c>
       <c r="F141" s="7" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="H141" s="7" t="s">
         <v>266</v>
       </c>
       <c r="I141" s="7" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8293,28 +8309,28 @@
         <v>141</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="E142" s="7" t="s">
         <v>191</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>842</v>
+        <v>833</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="H142" s="7" t="s">
         <v>270</v>
       </c>
       <c r="I142" s="7" t="s">
-        <v>761</v>
+        <v>752</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8322,28 +8338,28 @@
         <v>142</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="E143" s="7" t="s">
         <v>196</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>841</v>
+        <v>832</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="H143" s="7" t="s">
         <v>274</v>
       </c>
       <c r="I143" s="7" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -8351,28 +8367,28 @@
         <v>143</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="E144" s="7" t="s">
         <v>201</v>
       </c>
       <c r="F144" s="7" t="s">
-        <v>764</v>
+        <v>755</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="H144" s="7" t="s">
         <v>203</v>
       </c>
       <c r="I144" s="7" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -8380,28 +8396,28 @@
         <v>144</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>280</v>
       </c>
       <c r="F145" s="7" t="s">
-        <v>767</v>
+        <v>758</v>
       </c>
       <c r="G145" s="6" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="H145" s="7" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="I145" s="7" t="s">
-        <v>766</v>
+        <v>757</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8409,28 +8425,28 @@
         <v>145</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>285</v>
       </c>
       <c r="F146" s="7" t="s">
-        <v>768</v>
+        <v>759</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="H146" s="7" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="I146" s="7" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -8438,28 +8454,28 @@
         <v>146</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>290</v>
       </c>
       <c r="F147" s="7" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8467,28 +8483,28 @@
         <v>147</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="E148" s="7" t="s">
         <v>221</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="H148" s="7" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="I148" s="7" t="s">
-        <v>773</v>
+        <v>764</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -8496,13 +8512,13 @@
         <v>148</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="E149" s="7" t="s">
         <v>226</v>
@@ -8511,10 +8527,10 @@
         <v>227</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="I149" s="6" t="s">
         <v>230</v>
@@ -8525,7 +8541,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>303</v>
@@ -8534,7 +8550,7 @@
         <v>304</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>878</v>
+        <v>868</v>
       </c>
       <c r="F150" s="6" t="s">
         <v>305</v>
@@ -8554,7 +8570,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>309</v>
@@ -8563,7 +8579,7 @@
         <v>310</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>879</v>
+        <v>869</v>
       </c>
       <c r="F151" s="6" t="s">
         <v>309</v>
@@ -8583,28 +8599,28 @@
         <v>151</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>689</v>
+        <v>872</v>
       </c>
       <c r="E152" s="7" t="s">
-        <v>690</v>
+        <v>681</v>
       </c>
       <c r="F152" s="7" t="s">
-        <v>840</v>
+        <v>831</v>
       </c>
       <c r="G152" s="6" t="s">
-        <v>691</v>
+        <v>682</v>
       </c>
       <c r="H152" s="7" t="s">
-        <v>692</v>
+        <v>683</v>
       </c>
       <c r="I152" s="7" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -8612,28 +8628,28 @@
         <v>152</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>693</v>
+        <v>684</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>694</v>
+        <v>685</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="G153" s="6" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="H153" s="7" t="s">
-        <v>696</v>
+        <v>687</v>
       </c>
       <c r="I153" s="7" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -8641,28 +8657,28 @@
         <v>153</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
       <c r="E154" s="7" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>838</v>
+        <v>829</v>
       </c>
       <c r="G154" s="6" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
       <c r="H154" s="7" t="s">
-        <v>701</v>
+        <v>692</v>
       </c>
       <c r="I154" s="7" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -8670,28 +8686,28 @@
         <v>154</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>702</v>
+        <v>693</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>881</v>
+        <v>871</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>837</v>
+        <v>828</v>
       </c>
       <c r="G155" s="6" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
       <c r="H155" s="7" t="s">
-        <v>705</v>
+        <v>696</v>
       </c>
       <c r="I155" s="7" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -8699,28 +8715,28 @@
         <v>155</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C156" s="6" t="s">
         <v>298</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
       <c r="E156" s="7" t="s">
         <v>300</v>
       </c>
       <c r="F156" s="7" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
       <c r="G156" s="6" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
       <c r="H156" s="7" t="s">
-        <v>708</v>
+        <v>699</v>
       </c>
       <c r="I156" s="7" t="s">
-        <v>833</v>
+        <v>824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>